<commit_message>
Fixed the bar color alteration
</commit_message>
<xml_diff>
--- a/backend/expense.xlsx
+++ b/backend/expense.xlsx
@@ -462,10 +462,10 @@
         <v>Movie</v>
       </c>
       <c r="B6">
-        <v>750</v>
+        <v>760</v>
       </c>
       <c r="C6" t="str">
-        <v>4/5/2025</v>
+        <v>4/9/2025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>